<commit_message>
w1 practice problems excel
</commit_message>
<xml_diff>
--- a/w1/SC2x_W1L1_IntroNetworkDesign.xlsx
+++ b/w1/SC2x_W1L1_IntroNetworkDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/caroline_c_barbosa_accenture_com/Documents/Desktop/06_cursos/SCM/SC2x/w1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="334" documentId="11_7CC71676DD3CE230A0165AF3277EF0E787C263A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA106A5-421C-4621-BBD8-20657CA54DA3}"/>
+  <xr:revisionPtr revIDLastSave="827" documentId="11_7CC71676DD3CE230A0165AF3277EF0E787C263A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CB763DC-44DB-4749-AE63-600542299AA0}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="348" windowWidth="17484" windowHeight="10296" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SandyCoPART1 v1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="SandyCo PART2" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SandyCo PART2'!$A$3:$Q$10</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">'SandyCo PART2'!$C$5:$L$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SandyCo PART2'!$A$3:$R$10</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'SandyCo PART2'!$C$5:$M$5</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'SandyCoPART1 v1'!$C$5:$H$5</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'SandyCoPART1 v2'!$C$5:$E$6</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'SandyCoPART1 v3'!$C$5:$E$6</definedName>
@@ -46,15 +46,16 @@
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'SandyCoPART1 v1'!$C$5:$H$5</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'SandyCoPART1 v2'!$C$13:$C$14</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'SandyCoPART1 v3'!$C$5:$E$6</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'SandyCo PART2'!$M$13:$M$15</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'SandyCo PART2'!$N$13:$N$15</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'SandyCoPART1 v1'!$I$13:$I$15</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'SandyCoPART1 v2'!$C$17:$C$19</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'SandyCoPART1 v3'!$C$7:$E$7</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'SandyCo PART2'!$M$18:$M$19</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'SandyCo PART2'!$N$18:$N$19</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'SandyCoPART1 v1'!$I$9:$I$10</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">'SandyCoPART1 v2'!$C$5:$E$6</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'SandyCoPART1 v3'!$F$5:$F$6</definedName>
-    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'SandyCo PART2'!$M$9:$M$10</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'SandyCo PART2'!$N$24</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">'SandyCo PART2'!$N$9:$N$10</definedName>
     <definedName name="solver_lin" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
@@ -83,7 +84,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">3</definedName>
@@ -114,19 +115,21 @@
     <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'SandyCoPART1 v2'!$E$13:$E$14</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'SandyCo PART2'!$O$13:$O$15</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'SandyCo PART2'!$P$13:$P$15</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'SandyCoPART1 v1'!$K$13:$K$15</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">'SandyCoPART1 v2'!$E$17:$E$19</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'SandyCoPART1 v3'!$C$8:$E$8</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'SandyCo PART2'!$O$18:$O$19</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'SandyCo PART2'!$P$18:$P$19</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'SandyCoPART1 v1'!$K$9:$K$10</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'SandyCoPART1 v3'!$G$5:$G$6</definedName>
-    <definedName name="solver_rhs4" localSheetId="3" hidden="1">'SandyCo PART2'!$O$9:$O$10</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">'SandyCo PART2'!$P$24</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">'SandyCo PART2'!$P$9:$P$10</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
@@ -165,10 +168,10 @@
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -192,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="44">
   <si>
     <t xml:space="preserve">z = </t>
   </si>
@@ -318,6 +321,12 @@
   </si>
   <si>
     <t>SandyCo - Alternative Spreadsheet FORMULATION 3</t>
+  </si>
+  <si>
+    <t>DC_capacity</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -583,6 +592,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -638,7 +676,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -729,6 +767,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1123,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1377,7 +1427,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1604,7 +1656,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1778,34 +1830,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.796875" customWidth="1"/>
     <col min="3" max="11" width="5.5" style="4" customWidth="1"/>
-    <col min="12" max="13" width="5.5" customWidth="1"/>
-    <col min="14" max="14" width="2.19921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="5.5" customWidth="1"/>
+    <col min="15" max="15" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.69921875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="16">
-        <f>SUMPRODUCT(C5:L5,C6:L6)</f>
-        <v>69200</v>
+        <f>SUMPRODUCT(C5:M5,C6:M6)</f>
+        <v>66675</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>32</v>
@@ -1821,8 +1873,9 @@
       <c r="J3" s="34"/>
       <c r="K3" s="34"/>
       <c r="L3" s="35"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C4" s="19" t="s">
         <v>22</v>
       </c>
@@ -1853,54 +1906,60 @@
       <c r="L4" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M4" s="36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="21">
+        <v>95</v>
+      </c>
+      <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="3">
-        <v>75</v>
-      </c>
       <c r="E5" s="3">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F5" s="22">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="G5" s="21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I5" s="3">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J5" s="3">
         <v>0</v>
       </c>
       <c r="K5" s="3">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="L5" s="22">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="19">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D6" s="2">
         <v>210</v>
       </c>
       <c r="E6" s="2">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="F6" s="20">
         <v>205</v>
@@ -1923,8 +1982,11 @@
       <c r="L6" s="20">
         <v>145</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M6" s="36">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
       <c r="C7" s="23"/>
       <c r="D7" s="24"/>
@@ -1936,8 +1998,9 @@
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
       <c r="L7" s="29"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M7" s="37"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1952,15 +2015,16 @@
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
       <c r="L8" s="29"/>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="37"/>
+      <c r="N8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="13" t="s">
+      <c r="O8" s="4"/>
+      <c r="P8" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
@@ -1978,18 +2042,19 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="30"/>
-      <c r="M9" s="6">
-        <f>SUMPRODUCT(C9:L9,$C$5:$L$5)</f>
-        <v>75</v>
-      </c>
-      <c r="N9" s="2" t="s">
+      <c r="M9" s="38"/>
+      <c r="N9" s="6">
+        <f>SUMPRODUCT(C9:M9,$C$5:$M$5)</f>
+        <v>95</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
         <v>9</v>
       </c>
@@ -2007,18 +2072,21 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="30"/>
-      <c r="M10" s="6">
-        <f>SUMPRODUCT(C10:L10,$C$5:$L$5)</f>
+      <c r="M10" s="38">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6">
+        <f>SUMPRODUCT(C10:M10,$C$5:$M$5)</f>
+        <v>105</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="5">
         <v>125</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O10" s="5">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="10"/>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
@@ -2030,10 +2098,11 @@
       <c r="J11" s="24"/>
       <c r="K11" s="24"/>
       <c r="L11" s="29"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="37"/>
       <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2048,10 +2117,11 @@
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="29"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="37"/>
       <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
         <v>11</v>
       </c>
@@ -2069,18 +2139,21 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="20"/>
-      <c r="M13" s="6">
-        <f>SUMPRODUCT(C13:L13,$C$5:$L$5)</f>
+      <c r="M13" s="39">
+        <v>1</v>
+      </c>
+      <c r="N13" s="6">
+        <f>SUMPRODUCT(C13:M13,$C$5:$M$5)</f>
         <v>25</v>
       </c>
-      <c r="N13" s="2" t="s">
+      <c r="O13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
         <v>12</v>
       </c>
@@ -2098,18 +2171,19 @@
         <v>1</v>
       </c>
       <c r="L14" s="20"/>
-      <c r="M14" s="6">
-        <f>SUMPRODUCT(C14:L14,$C$5:$L$5)</f>
+      <c r="M14" s="39"/>
+      <c r="N14" s="6">
+        <f t="shared" ref="N14:N15" si="0">SUMPRODUCT(C14:M14,$C$5:$M$5)</f>
         <v>95</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
         <v>13</v>
       </c>
@@ -2127,18 +2201,19 @@
       <c r="L15" s="20">
         <v>1</v>
       </c>
-      <c r="M15" s="6">
-        <f>SUMPRODUCT(C15:L15,$C$5:$L$5)</f>
+      <c r="M15" s="39"/>
+      <c r="N15" s="6">
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="O15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C16" s="23"/>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
@@ -2149,8 +2224,9 @@
       <c r="J16" s="24"/>
       <c r="K16" s="24"/>
       <c r="L16" s="29"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M16" s="37"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2164,8 +2240,9 @@
       <c r="J17" s="24"/>
       <c r="K17" s="24"/>
       <c r="L17" s="29"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M17" s="37"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
         <v>35</v>
       </c>
@@ -2189,18 +2266,19 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="30"/>
-      <c r="M18" s="6">
+      <c r="M18" s="38"/>
+      <c r="N18" s="6">
         <f>SUMPRODUCT(C18:L18,$C$5:$L$5)</f>
         <v>0</v>
       </c>
-      <c r="N18" s="15" t="s">
+      <c r="O18" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="O18" s="2">
+      <c r="P18" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="18" t="s">
         <v>36</v>
       </c>
@@ -2224,15 +2302,47 @@
       <c r="L19" s="31">
         <v>-1</v>
       </c>
-      <c r="M19" s="6">
+      <c r="M19" s="40"/>
+      <c r="N19" s="6">
         <f>SUMPRODUCT(C19:L19,$C$5:$L$5)</f>
         <v>0</v>
       </c>
-      <c r="N19" s="15" t="s">
+      <c r="O19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="O19" s="2">
+      <c r="P19" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <f>SUMPRODUCT(C24:M24,C5:M5)</f>
+        <v>80</v>
+      </c>
+      <c r="O24" t="s">
+        <v>43</v>
+      </c>
+      <c r="P24" s="4">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>